<commit_message>
Commit with testing yatra flight booking
</commit_message>
<xml_diff>
--- a/YatraAutomation/src/test/resources/testData/testinput.xlsx
+++ b/YatraAutomation/src/test/resources/testData/testinput.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15885" windowHeight="5880" activeTab="1"/>
+    <workbookView windowWidth="16275" windowHeight="4845" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:B1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>hyderabad</t>
   </si>
@@ -24,12 +25,6 @@
     <t>kolkata</t>
   </si>
   <si>
-    <t>chennai</t>
-  </si>
-  <si>
-    <t>mumbai</t>
-  </si>
-  <si>
     <t>delhi</t>
   </si>
   <si>
@@ -58,6 +53,12 @@
   </si>
   <si>
     <t>chauhaninfj@gmail.com</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>dcbdcdcb</t>
   </si>
 </sst>
 </file>
@@ -65,9 +66,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -87,21 +88,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -117,7 +103,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -132,6 +118,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -139,9 +187,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,67 +223,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -232,31 +233,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,13 +365,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,133 +407,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,16 +431,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -459,17 +466,28 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,34 +510,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,15 +529,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,130 +547,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1002,15 +1003,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="10.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="12.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1035,22 +1036,6 @@
       </c>
       <c r="B3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1064,7 +1049,7 @@
   <sheetPr/>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -1076,22 +1061,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1101,4 +1086,29 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>